<commit_message>
[TRY] Filtros de mantenimiento
</commit_message>
<xml_diff>
--- a/Codigo_72_contratos.xlsx
+++ b/Codigo_72_contratos.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://potencia719-my.sharepoint.com/personal/practicante_potencia_com_co/Documents/Documents/TAREA_ENTIDADES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_784551B3D3B0527113DA2111595ED87656C87311" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_784551B3D3B0527113DA2111595ED87656C87311" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB77DB31-9A06-4047-B3D1-9C0C238E781C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1080" yWindow="504" windowWidth="17280" windowHeight="11736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$639</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -2312,6 +2315,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2599,13 +2606,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H639"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -13449,7 +13462,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>95</v>
       </c>
@@ -13475,7 +13488,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>95</v>
       </c>
@@ -13501,7 +13514,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>95</v>
       </c>
@@ -13527,7 +13540,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>95</v>
       </c>
@@ -13553,7 +13566,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>95</v>
       </c>
@@ -13579,7 +13592,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>95</v>
       </c>
@@ -13605,7 +13618,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>95</v>
       </c>
@@ -13631,7 +13644,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>95</v>
       </c>
@@ -13657,7 +13670,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>95</v>
       </c>
@@ -13683,7 +13696,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A427">
         <v>95</v>
       </c>
@@ -13709,7 +13722,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428">
         <v>95</v>
       </c>
@@ -13735,7 +13748,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A429">
         <v>95</v>
       </c>
@@ -13761,7 +13774,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A430">
         <v>95</v>
       </c>
@@ -13787,7 +13800,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A431">
         <v>95</v>
       </c>
@@ -13813,7 +13826,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A432">
         <v>95</v>
       </c>
@@ -13839,7 +13852,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A433">
         <v>95</v>
       </c>
@@ -13865,7 +13878,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A434">
         <v>95</v>
       </c>
@@ -13891,7 +13904,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A435">
         <v>95</v>
       </c>
@@ -13917,7 +13930,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A436">
         <v>95</v>
       </c>
@@ -13943,7 +13956,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437">
         <v>95</v>
       </c>
@@ -13969,7 +13982,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A438">
         <v>95</v>
       </c>
@@ -13995,7 +14008,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439">
         <v>95</v>
       </c>
@@ -14021,7 +14034,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A440">
         <v>95</v>
       </c>
@@ -14047,7 +14060,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A441">
         <v>95</v>
       </c>
@@ -14073,7 +14086,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A442">
         <v>95</v>
       </c>
@@ -14099,7 +14112,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A443">
         <v>95</v>
       </c>
@@ -14125,7 +14138,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A444">
         <v>95</v>
       </c>
@@ -14151,7 +14164,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A445">
         <v>95</v>
       </c>
@@ -14177,7 +14190,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A446">
         <v>95</v>
       </c>
@@ -14203,7 +14216,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A447">
         <v>95</v>
       </c>
@@ -14229,7 +14242,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="448" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A448">
         <v>95</v>
       </c>
@@ -14255,7 +14268,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="449" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A449">
         <v>95</v>
       </c>
@@ -14281,7 +14294,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="450" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A450">
         <v>95</v>
       </c>
@@ -14307,7 +14320,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="451" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A451">
         <v>95</v>
       </c>
@@ -14333,7 +14346,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="452" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A452">
         <v>95</v>
       </c>
@@ -14359,7 +14372,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="453" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A453">
         <v>95</v>
       </c>
@@ -14385,7 +14398,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="454" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A454">
         <v>95</v>
       </c>
@@ -14411,7 +14424,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="455" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A455">
         <v>95</v>
       </c>
@@ -14437,7 +14450,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="456" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A456">
         <v>95</v>
       </c>
@@ -14463,7 +14476,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="457" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A457">
         <v>95</v>
       </c>
@@ -14489,7 +14502,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="458" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A458">
         <v>95</v>
       </c>
@@ -14515,7 +14528,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="459" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A459">
         <v>95</v>
       </c>
@@ -14541,7 +14554,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="460" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A460">
         <v>95</v>
       </c>
@@ -14567,7 +14580,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="461" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A461">
         <v>95</v>
       </c>
@@ -14593,7 +14606,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="462" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A462">
         <v>95</v>
       </c>
@@ -14619,7 +14632,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="463" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A463">
         <v>95</v>
       </c>
@@ -14645,7 +14658,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="464" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A464">
         <v>95</v>
       </c>
@@ -14671,7 +14684,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="465" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A465">
         <v>95</v>
       </c>
@@ -14697,7 +14710,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="466" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A466">
         <v>95</v>
       </c>
@@ -14723,7 +14736,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="467" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A467">
         <v>95</v>
       </c>
@@ -14749,7 +14762,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="468" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A468">
         <v>95</v>
       </c>
@@ -14775,7 +14788,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="469" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A469">
         <v>95</v>
       </c>
@@ -14801,7 +14814,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="470" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A470">
         <v>95</v>
       </c>
@@ -14827,7 +14840,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="471" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A471">
         <v>95</v>
       </c>
@@ -14853,7 +14866,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="472" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A472">
         <v>95</v>
       </c>
@@ -14879,7 +14892,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="473" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A473">
         <v>95</v>
       </c>
@@ -14905,7 +14918,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="474" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A474">
         <v>95</v>
       </c>
@@ -14931,7 +14944,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="475" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A475">
         <v>95</v>
       </c>
@@ -14957,7 +14970,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="476" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A476">
         <v>95</v>
       </c>
@@ -14983,7 +14996,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="477" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A477">
         <v>95</v>
       </c>
@@ -15009,7 +15022,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="478" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A478">
         <v>95</v>
       </c>
@@ -15035,7 +15048,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="479" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A479">
         <v>95</v>
       </c>
@@ -15061,7 +15074,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="480" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A480">
         <v>95</v>
       </c>
@@ -15087,7 +15100,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="481" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A481">
         <v>95</v>
       </c>
@@ -15113,7 +15126,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="482" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A482">
         <v>95</v>
       </c>
@@ -15139,7 +15152,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="483" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A483">
         <v>95</v>
       </c>
@@ -15165,7 +15178,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="484" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A484">
         <v>95</v>
       </c>
@@ -15191,7 +15204,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="485" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A485">
         <v>95</v>
       </c>
@@ -15217,7 +15230,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="486" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A486">
         <v>95</v>
       </c>
@@ -15243,7 +15256,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="487" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A487">
         <v>95</v>
       </c>
@@ -15269,7 +15282,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="488" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A488">
         <v>95</v>
       </c>
@@ -15295,7 +15308,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="489" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A489">
         <v>95</v>
       </c>
@@ -15321,7 +15334,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="490" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A490">
         <v>95</v>
       </c>
@@ -15347,7 +15360,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="491" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A491">
         <v>95</v>
       </c>
@@ -15373,7 +15386,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="492" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492">
         <v>95</v>
       </c>
@@ -15399,7 +15412,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="493" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A493">
         <v>95</v>
       </c>
@@ -15425,7 +15438,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="494" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A494">
         <v>95</v>
       </c>
@@ -15451,7 +15464,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="495" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A495">
         <v>95</v>
       </c>
@@ -15477,7 +15490,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="496" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A496">
         <v>95</v>
       </c>
@@ -15503,7 +15516,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="497" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A497">
         <v>95</v>
       </c>
@@ -15529,7 +15542,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="498" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A498">
         <v>95</v>
       </c>
@@ -15555,7 +15568,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="499" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A499">
         <v>95</v>
       </c>
@@ -15581,7 +15594,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="500" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A500">
         <v>95</v>
       </c>
@@ -15607,7 +15620,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="501" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A501">
         <v>95</v>
       </c>
@@ -15633,7 +15646,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="502" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A502">
         <v>95</v>
       </c>
@@ -15659,7 +15672,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="503" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A503">
         <v>95</v>
       </c>
@@ -15685,7 +15698,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="504" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A504">
         <v>95</v>
       </c>
@@ -15711,7 +15724,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="505" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A505">
         <v>95</v>
       </c>
@@ -15737,7 +15750,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="506" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A506">
         <v>95</v>
       </c>
@@ -15763,7 +15776,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="507" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A507">
         <v>95</v>
       </c>
@@ -15789,7 +15802,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="508" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A508">
         <v>95</v>
       </c>
@@ -15815,7 +15828,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="509" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A509">
         <v>95</v>
       </c>
@@ -15841,7 +15854,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="510" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A510">
         <v>95</v>
       </c>
@@ -15867,7 +15880,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="511" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A511">
         <v>95</v>
       </c>
@@ -15893,7 +15906,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="512" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A512">
         <v>95</v>
       </c>
@@ -15919,7 +15932,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="513" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A513">
         <v>95</v>
       </c>
@@ -15945,7 +15958,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="514" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A514">
         <v>95</v>
       </c>
@@ -15971,7 +15984,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="515" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A515">
         <v>95</v>
       </c>
@@ -15997,7 +16010,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="516" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A516">
         <v>95</v>
       </c>
@@ -16023,7 +16036,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="517" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A517">
         <v>95</v>
       </c>
@@ -16049,7 +16062,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="518" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A518">
         <v>95</v>
       </c>
@@ -16075,7 +16088,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="519" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A519">
         <v>95</v>
       </c>
@@ -16101,7 +16114,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="520" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A520">
         <v>95</v>
       </c>
@@ -16127,7 +16140,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="521" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A521">
         <v>95</v>
       </c>
@@ -16153,7 +16166,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="522" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A522">
         <v>95</v>
       </c>
@@ -16179,7 +16192,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="523" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A523">
         <v>95</v>
       </c>
@@ -16205,7 +16218,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="524" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A524">
         <v>95</v>
       </c>
@@ -16231,7 +16244,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="525" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A525">
         <v>95</v>
       </c>
@@ -16257,7 +16270,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="526" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A526">
         <v>95</v>
       </c>
@@ -16283,7 +16296,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="527" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="527" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A527">
         <v>95</v>
       </c>
@@ -16309,7 +16322,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="528" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A528">
         <v>95</v>
       </c>
@@ -16335,7 +16348,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="529" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A529">
         <v>95</v>
       </c>
@@ -16361,7 +16374,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="530" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A530">
         <v>95</v>
       </c>
@@ -16387,7 +16400,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="531" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A531">
         <v>95</v>
       </c>
@@ -16413,7 +16426,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="532" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A532">
         <v>95</v>
       </c>
@@ -16439,7 +16452,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="533" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A533">
         <v>95</v>
       </c>
@@ -16465,7 +16478,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="534" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A534">
         <v>95</v>
       </c>
@@ -16491,7 +16504,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="535" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A535">
         <v>95</v>
       </c>
@@ -16517,7 +16530,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="536" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A536">
         <v>95</v>
       </c>
@@ -16543,7 +16556,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="537" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A537">
         <v>95</v>
       </c>
@@ -16569,7 +16582,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="538" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A538">
         <v>95</v>
       </c>
@@ -16595,7 +16608,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="539" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A539">
         <v>95</v>
       </c>
@@ -16621,7 +16634,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="540" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A540">
         <v>95</v>
       </c>
@@ -16647,7 +16660,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="541" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A541">
         <v>95</v>
       </c>
@@ -16673,7 +16686,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="542" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A542">
         <v>95</v>
       </c>
@@ -16699,7 +16712,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="543" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A543">
         <v>95</v>
       </c>
@@ -16725,7 +16738,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="544" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A544">
         <v>95</v>
       </c>
@@ -16751,7 +16764,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="545" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A545">
         <v>95</v>
       </c>
@@ -16777,7 +16790,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="546" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A546">
         <v>95</v>
       </c>
@@ -16803,7 +16816,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="547" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A547">
         <v>95</v>
       </c>
@@ -16829,7 +16842,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="548" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A548">
         <v>95</v>
       </c>
@@ -16855,7 +16868,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="549" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A549">
         <v>95</v>
       </c>
@@ -16881,7 +16894,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="550" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A550">
         <v>95</v>
       </c>
@@ -16907,7 +16920,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="551" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A551">
         <v>95</v>
       </c>
@@ -16933,7 +16946,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="552" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A552">
         <v>95</v>
       </c>
@@ -16959,7 +16972,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="553" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A553">
         <v>95</v>
       </c>
@@ -16985,7 +16998,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="554" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A554">
         <v>95</v>
       </c>
@@ -17011,7 +17024,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="555" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A555">
         <v>95</v>
       </c>
@@ -17037,7 +17050,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="556" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A556">
         <v>95</v>
       </c>
@@ -17063,7 +17076,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="557" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A557">
         <v>95</v>
       </c>
@@ -17089,7 +17102,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="558" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A558">
         <v>95</v>
       </c>
@@ -17115,7 +17128,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="559" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A559">
         <v>95</v>
       </c>
@@ -17141,7 +17154,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="560" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A560">
         <v>95</v>
       </c>
@@ -17167,7 +17180,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="561" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A561">
         <v>95</v>
       </c>
@@ -17193,7 +17206,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="562" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A562">
         <v>95</v>
       </c>
@@ -17219,7 +17232,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="563" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A563">
         <v>95</v>
       </c>
@@ -17245,7 +17258,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="564" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="564" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A564">
         <v>95</v>
       </c>
@@ -17271,7 +17284,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="565" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A565">
         <v>95</v>
       </c>
@@ -17297,7 +17310,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="566" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A566">
         <v>95</v>
       </c>
@@ -17323,7 +17336,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="567" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A567">
         <v>95</v>
       </c>
@@ -17349,7 +17362,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="568" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A568">
         <v>95</v>
       </c>
@@ -17375,7 +17388,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="569" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A569">
         <v>95</v>
       </c>
@@ -17401,7 +17414,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="570" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A570">
         <v>95</v>
       </c>
@@ -17427,7 +17440,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="571" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A571">
         <v>95</v>
       </c>
@@ -17453,7 +17466,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="572" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A572">
         <v>95</v>
       </c>
@@ -17479,7 +17492,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="573" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A573">
         <v>95</v>
       </c>
@@ -17505,7 +17518,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="574" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A574">
         <v>95</v>
       </c>
@@ -17531,7 +17544,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="575" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A575">
         <v>95</v>
       </c>
@@ -17557,7 +17570,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="576" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A576">
         <v>95</v>
       </c>
@@ -17583,7 +17596,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="577" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A577">
         <v>95</v>
       </c>
@@ -17609,7 +17622,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="578" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A578">
         <v>95</v>
       </c>
@@ -17635,7 +17648,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="579" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A579">
         <v>95</v>
       </c>
@@ -17661,7 +17674,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="580" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A580">
         <v>95</v>
       </c>
@@ -17687,7 +17700,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="581" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A581">
         <v>95</v>
       </c>
@@ -17713,7 +17726,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="582" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A582">
         <v>95</v>
       </c>
@@ -17739,7 +17752,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="583" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A583">
         <v>95</v>
       </c>
@@ -17765,7 +17778,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="584" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A584">
         <v>95</v>
       </c>
@@ -17791,7 +17804,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="585" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A585">
         <v>95</v>
       </c>
@@ -17817,7 +17830,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="586" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A586">
         <v>95</v>
       </c>
@@ -17843,7 +17856,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="587" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A587">
         <v>95</v>
       </c>
@@ -17869,7 +17882,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="588" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A588">
         <v>95</v>
       </c>
@@ -17895,7 +17908,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="589" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A589">
         <v>95</v>
       </c>
@@ -17921,7 +17934,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="590" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A590">
         <v>95</v>
       </c>
@@ -17947,7 +17960,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="591" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A591">
         <v>95</v>
       </c>
@@ -17973,7 +17986,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="592" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A592">
         <v>95</v>
       </c>
@@ -17999,7 +18012,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="593" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A593">
         <v>95</v>
       </c>
@@ -18025,7 +18038,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="594" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A594">
         <v>95</v>
       </c>
@@ -18051,7 +18064,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="595" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A595">
         <v>95</v>
       </c>
@@ -18077,7 +18090,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="596" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A596">
         <v>95</v>
       </c>
@@ -18103,7 +18116,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="597" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A597">
         <v>95</v>
       </c>
@@ -18129,7 +18142,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="598" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A598">
         <v>95</v>
       </c>
@@ -18155,7 +18168,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="599" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A599">
         <v>95</v>
       </c>
@@ -18181,7 +18194,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="600" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A600">
         <v>95</v>
       </c>
@@ -18207,7 +18220,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="601" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A601">
         <v>95</v>
       </c>
@@ -18233,7 +18246,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="602" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A602">
         <v>95</v>
       </c>
@@ -18259,7 +18272,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="603" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="603" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A603">
         <v>95</v>
       </c>
@@ -18285,7 +18298,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="604" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A604">
         <v>95</v>
       </c>
@@ -18311,7 +18324,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="605" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A605">
         <v>95</v>
       </c>
@@ -18337,7 +18350,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="606" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="606" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A606">
         <v>95</v>
       </c>
@@ -18363,7 +18376,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="607" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A607">
         <v>95</v>
       </c>
@@ -18389,7 +18402,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="608" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A608">
         <v>95</v>
       </c>
@@ -18415,7 +18428,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="609" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="609" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A609">
         <v>95</v>
       </c>
@@ -18441,7 +18454,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="610" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="610" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A610">
         <v>95</v>
       </c>
@@ -18467,7 +18480,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="611" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="611" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A611">
         <v>95</v>
       </c>
@@ -18493,7 +18506,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="612" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="612" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A612">
         <v>95</v>
       </c>
@@ -18519,7 +18532,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="613" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="613" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A613">
         <v>95</v>
       </c>
@@ -18545,7 +18558,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="614" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="614" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A614">
         <v>95</v>
       </c>
@@ -18571,7 +18584,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="615" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="615" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A615">
         <v>95</v>
       </c>
@@ -18597,7 +18610,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="616" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="616" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A616">
         <v>95</v>
       </c>
@@ -18623,7 +18636,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="617" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="617" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A617">
         <v>95</v>
       </c>
@@ -18649,7 +18662,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="618" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="618" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A618">
         <v>95</v>
       </c>
@@ -18675,7 +18688,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="619" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="619" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A619">
         <v>95</v>
       </c>
@@ -18701,7 +18714,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="620" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="620" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A620">
         <v>95</v>
       </c>
@@ -18727,7 +18740,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="621" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="621" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A621">
         <v>95</v>
       </c>
@@ -18753,7 +18766,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="622" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="622" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A622">
         <v>95</v>
       </c>
@@ -18779,7 +18792,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="623" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="623" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A623">
         <v>95</v>
       </c>
@@ -18805,7 +18818,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="624" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="624" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A624">
         <v>95</v>
       </c>
@@ -18831,7 +18844,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="625" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="625" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A625">
         <v>95</v>
       </c>
@@ -18857,7 +18870,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="626" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="626" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A626">
         <v>95</v>
       </c>
@@ -18883,7 +18896,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="627" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="627" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A627">
         <v>95</v>
       </c>
@@ -18909,7 +18922,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="628" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="628" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A628">
         <v>95</v>
       </c>
@@ -18935,7 +18948,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="629" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="629" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A629">
         <v>95</v>
       </c>
@@ -18961,7 +18974,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="630" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="630" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A630">
         <v>95</v>
       </c>
@@ -18987,7 +19000,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="631" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="631" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A631">
         <v>95</v>
       </c>
@@ -19013,7 +19026,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="632" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="632" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A632">
         <v>95</v>
       </c>
@@ -19039,7 +19052,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="633" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="633" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A633">
         <v>95</v>
       </c>
@@ -19065,7 +19078,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="634" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="634" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A634">
         <v>95</v>
       </c>
@@ -19091,7 +19104,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="635" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="635" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A635">
         <v>95</v>
       </c>
@@ -19117,7 +19130,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="636" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="636" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A636">
         <v>95</v>
       </c>
@@ -19143,7 +19156,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="637" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="637" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A637">
         <v>95</v>
       </c>
@@ -19169,7 +19182,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="638" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="638" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A638">
         <v>95</v>
       </c>
@@ -19195,7 +19208,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="639" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="639" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A639">
         <v>95</v>
       </c>
@@ -19222,6 +19235,17 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H639" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="7210"/>
+        <filter val="7211"/>
+        <filter val="7212"/>
+        <filter val="7214"/>
+        <filter val="7215"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>